<commit_message>
Daily_Scrum, Fejlesztési dokumentáció fejlesztése
</commit_message>
<xml_diff>
--- a/Daily_Scrum.xlsx
+++ b/Daily_Scrum.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gitrepo\11E-weboldal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\11E-weboldal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF7A53F-DB36-4611-B4EC-C36BCFF105F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FAEFB1-47BF-450F-98D2-EC4AE3E512D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Tomó Zalán, Nagy Ákos, Chen Haole, Fehér Szabolcs Napi Scrum</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Órarend beillesztése, linkelés</t>
   </si>
   <si>
-    <t>Nem volt elérhető a github repo</t>
-  </si>
-  <si>
     <t>Tantárgy kártya sablom (matek), CSS</t>
   </si>
   <si>
@@ -106,6 +103,12 @@
   </si>
   <si>
     <t>Fejlesztési dokumentáció fejlesztése, csapat segítése, scrum</t>
+  </si>
+  <si>
+    <t>Tanár lehetetlen időkeretet adott</t>
+  </si>
+  <si>
+    <t>Nem volt elérhető a github repo, Tanár lehetetlen időkeretet adott</t>
   </si>
 </sst>
 </file>
@@ -299,28 +302,28 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -608,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,152 +625,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="9">
         <v>45932</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="11">
         <v>45937</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scrum dokumentáció 1 fejlesztése, forras.txt hozzáadása, Daily_Scrum.xlsx befejezése
</commit_message>
<xml_diff>
--- a/Daily_Scrum.xlsx
+++ b/Daily_Scrum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\11E-weboldal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Oskola dolgok\IKT\11E-weboldal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FAEFB1-47BF-450F-98D2-EC4AE3E512D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9306BC-6347-43CA-9365-023DD714E408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Tomó Zalán, Nagy Ákos, Chen Haole, Fehér Szabolcs Napi Scrum</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Chen Haole</t>
   </si>
   <si>
-    <t>Mit csináltam ma</t>
-  </si>
-  <si>
     <t>Mit fogok csinálni legközelebb</t>
   </si>
   <si>
@@ -108,7 +105,25 @@
     <t>Tanár lehetetlen időkeretet adott</t>
   </si>
   <si>
-    <t>Nem volt elérhető a github repo, Tanár lehetetlen időkeretet adott</t>
+    <t>2025.10.07  "8:55"</t>
+  </si>
+  <si>
+    <t>2025.10.07  "16:00"</t>
+  </si>
+  <si>
+    <t>angol, nemet.html hozzáadása, Daily Scrum, Fejlesztési dok. Scrum doc. Hozzáadása, PPT elkészítése</t>
+  </si>
+  <si>
+    <t>ABSZL HALL1-2 ASZAF.html hozzáadása</t>
+  </si>
+  <si>
+    <t>TESI WEBPROG SZAN.html hozzáadása</t>
+  </si>
+  <si>
+    <t>ABSZL HÁLL ASZAF.html hozzáadása</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -138,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -296,11 +311,212 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -309,19 +525,54 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -609,48 +860,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="49.140625" customWidth="1"/>
-    <col min="3" max="3" width="54.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" customWidth="1"/>
+    <col min="4" max="4" width="76.5703125" customWidth="1"/>
     <col min="5" max="5" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>45932</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -667,7 +917,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -682,7 +932,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -697,87 +947,140 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>45937</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>26</v>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="26"/>
+      <c r="E14" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="6">
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
PPT kész, eltérések kijavítása
</commit_message>
<xml_diff>
--- a/Daily_Scrum.xlsx
+++ b/Daily_Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Oskola dolgok\IKT\11E-weboldal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9306BC-6347-43CA-9365-023DD714E408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1539D66-8981-4C04-BF18-115C2DFF2720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Tomó Zalán, Nagy Ákos, Chen Haole, Fehér Szabolcs Napi Scrum</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Mit csináltam ma</t>
   </si>
 </sst>
 </file>
@@ -525,44 +528,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -863,7 +866,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,13 +879,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -891,7 +894,9 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
@@ -900,7 +905,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="16">
         <v>45932</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -917,7 +922,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -932,7 +937,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -947,22 +952,22 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -979,7 +984,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -994,7 +999,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1009,7 +1014,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
@@ -1024,16 +1029,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="24" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="27" t="s">
@@ -1041,33 +1046,33 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="28"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="26"/>

</xml_diff>